<commit_message>
Add submission info to export
</commit_message>
<xml_diff>
--- a/VKGL/scripts/clinvar_export/clinvar_template.xlsx
+++ b/VKGL/scripts/clinvar_export/clinvar_template.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-20880" yWindow="-18820" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="READ_ME" sheetId="1" r:id="rId1"/>
-    <sheet name="Variant" sheetId="2" r:id="rId2"/>
-    <sheet name="ExpEvidence" sheetId="3" r:id="rId3"/>
-    <sheet name="Deletes" sheetId="4" r:id="rId4"/>
+    <sheet name="SubmissionInfo" sheetId="5" r:id="rId2"/>
+    <sheet name="Variant" sheetId="2" r:id="rId3"/>
+    <sheet name="ExpEvidence" sheetId="3" r:id="rId4"/>
+    <sheet name="Deletes" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="195">
   <si>
     <t>For variants defined by sequence, provide an HGVS expression in this column. For variants defined cytogenetically, enter "cytogenetic"  in this column and the description (e.g. 11q14.3 deletion) in the Location column.</t>
   </si>
@@ -475,6 +476,314 @@
   <si>
     <t>Optional. You can provide a public comment explaining why this interpretation is being deleted.</t>
   </si>
+  <si>
+    <t>#Spreadsheet for submitting summary data to ClinVar.  This spreadsheet does not support all the data elements in ClinVar; if you wish to submit more detailed information please review our other submission spreadsheet.</t>
+  </si>
+  <si>
+    <t>Version L1.5</t>
+  </si>
+  <si>
+    <t>Release date 4/28/2016</t>
+  </si>
+  <si>
+    <t>Submission info - for columns U-AB, please fill in a single row with data that applies to the whole submission.</t>
+  </si>
+  <si>
+    <t>SubmitterID</t>
+  </si>
+  <si>
+    <t>SubmitterIDType</t>
+  </si>
+  <si>
+    <t>Submitter type</t>
+  </si>
+  <si>
+    <t>Submitter first name</t>
+  </si>
+  <si>
+    <t>Submitter last name</t>
+  </si>
+  <si>
+    <t>Submitter phone</t>
+  </si>
+  <si>
+    <t>Submitter email</t>
+  </si>
+  <si>
+    <t>Submitter role</t>
+  </si>
+  <si>
+    <t>Organization type</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>OrganizationID</t>
+  </si>
+  <si>
+    <t>Organization abbreviation</t>
+  </si>
+  <si>
+    <t>Organization URL</t>
+  </si>
+  <si>
+    <t>Institution</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State/Province</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Postal code</t>
+  </si>
+  <si>
+    <t>Primary organization</t>
+  </si>
+  <si>
+    <t>Submission name</t>
+  </si>
+  <si>
+    <t>Submission description</t>
+  </si>
+  <si>
+    <t>Study name</t>
+  </si>
+  <si>
+    <t>Review status</t>
+  </si>
+  <si>
+    <t>Release status</t>
+  </si>
+  <si>
+    <t>Submission date</t>
+  </si>
+  <si>
+    <t>Citation</t>
+  </si>
+  <si>
+    <t>Assembly name</t>
+  </si>
+  <si>
+    <t>Optional. Your  ClinVar/GTR PersonID, if you have submitted to ClinVar before, or your lab or organization's Handle, if you have submitted to dbSNP before. Otherwise, please leave this column blank.</t>
+  </si>
+  <si>
+    <t>Optional.The type of identifier provided in column A.  Allowed values currently are  Handle and ClinVar/GTR PersonID.</t>
+  </si>
+  <si>
+    <t>Required. The first name of the submitter.  This will be kept public or private, as indicated in Submitter type.</t>
+  </si>
+  <si>
+    <t>Required. The last name of submitter.  This will be kept public or private, as indicated in Submitter type.</t>
+  </si>
+  <si>
+    <t>Required. The phone number of the submitter. This will be kept public or private, as indicated in Submitter type.</t>
+  </si>
+  <si>
+    <t>Required. The email address of the submitter. This will be kept public or private, as indicated in Submitter type.</t>
+  </si>
+  <si>
+    <t>Required but only for public submitters. The submitter's role within the submitting organization. Note that here, "Contact" is the person that ClinVar users may contact with questions. This person may be the same as or different from the ClinVar contact, indicated in column C.</t>
+  </si>
+  <si>
+    <t>Required. Indicate the appropriate category for your organization: lab, LSDB, clinic, resource, consortium, other.</t>
+  </si>
+  <si>
+    <t>Required. Name of your lab or organization.</t>
+  </si>
+  <si>
+    <t>Optional identifier for your organization in GTR/ClinVar.  Applicable if your group has submitted to GTR or ClinVar previously. Note that this identifier is an integer, not the GTRL identifier from GTR.</t>
+  </si>
+  <si>
+    <t>Required. An abbreviation for your organization, suitable for display on webpages. This abbreviation must be unique, so ClinVar staff may work with you to determine an abbreviation that is both appropriate and unique.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional. The URL for your organization's website/homepage. </t>
+  </si>
+  <si>
+    <t>Required. The name of a larger institution that your organization or lab is part of.</t>
+  </si>
+  <si>
+    <t>Optional. Mailing address building/ street.  Up to 3 address lines can be separated by a semicolon.</t>
+  </si>
+  <si>
+    <t>Required if OrganizationID or SubmitterID Handle is not provided: Mailing address city</t>
+  </si>
+  <si>
+    <t>Required if OrganizationID or SubmitterID Handle is not provided and if it is applicable for the submitter's country: Mailing address state or province</t>
+  </si>
+  <si>
+    <t>Required if OrganizationID or SubmitterID Handle is not provided: Mailing address country</t>
+  </si>
+  <si>
+    <t>Optional. Mailing address postal code</t>
+  </si>
+  <si>
+    <t>Required if more than one organization is provided. Please enter "primary" for the *one* organization that should be considered primary for display on the ClinVar website.</t>
+  </si>
+  <si>
+    <t>Optional.  Free text to describe this submission. The submission description may be a sentence or short paragraph.</t>
+  </si>
+  <si>
+    <t>Optional. This allows a temporary hold on data being presented publicly. Allowed values are public or hold until published. If not supplied, public will be the default.</t>
+  </si>
+  <si>
+    <t>Optional.  If not provided, the date the file was received will be used. Use the format mm/dd/yyyy.</t>
+  </si>
+  <si>
+    <t>Optional. Citation for the complete submission. Will be represented as if submitted on the Variant tab and the ExpEvidence tab. PubMed ID, in the format PMID:123456.</t>
+  </si>
+  <si>
+    <t>Required. The genome assembly that was used to call variants in this submission. All variants in this file should use the same genome assembly. Allowed values: NCBI36, hg18, GRCh37, hg19, GRCh38, hg38.</t>
+  </si>
+  <si>
+    <t>#Examples are provided in lines 9-10.  Please start your submission in line 11.</t>
+  </si>
+  <si>
+    <t>EXAMPLE: MY_HANDLE_NAME</t>
+  </si>
+  <si>
+    <t>Handle</t>
+  </si>
+  <si>
+    <t>Contact; Public</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Doe</t>
+  </si>
+  <si>
+    <t>301-999-9999</t>
+  </si>
+  <si>
+    <t>john.doe@email.address</t>
+  </si>
+  <si>
+    <t>Laboratory director</t>
+  </si>
+  <si>
+    <t>Genetic Testing Lab</t>
+  </si>
+  <si>
+    <t>Some University Hospital</t>
+  </si>
+  <si>
+    <t>Clinical Bldg, Rm 100; 80 King Street West</t>
+  </si>
+  <si>
+    <t>Metropolis</t>
+  </si>
+  <si>
+    <t>Alberta</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>ON M5X 1A9</t>
+  </si>
+  <si>
+    <t>classified by single submitter</t>
+  </si>
+  <si>
+    <t>GRCh37</t>
+  </si>
+  <si>
+    <t>EXAMPLE: 25</t>
+  </si>
+  <si>
+    <t>PersonID</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Note that if you submit this file through the Submission Portal, we will use the submitter information in the portal, and ignore the information in this tab. Please visit the Submission Portal if you need to update your submitter information.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Submitter info - for columns A-Q, multiple rows may be filled in to provide information for each submitter for this submission.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Required. One and only one submitter must be the Contact, i.e. the individual to be contacted by ClinVar staff with questions about the content of the submission. The Contact’s information is private by default; if it should be public, use Contact, Public.
+Additional submitters may also be provided. Use Public for submitters who should be listed publicly as the source of information; otherwise, submit as Private.  
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Required if either Submission description or study name is provided. The name for this batch of submitted interpretations. This name will be indexed for searching ClinVar's website. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>NOTE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> To be compatible with current processing in dbSNP, a submission name must be different for every batch submitted using the same HANDLE. Please make sure the name is a single word; if it is must be more than a single word, separate the words with an underscore '_ '. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Optional.  To be used if the data are submitted as part of a named study,</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> e.g. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Framingham. The study name should be short and specific.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional. Level of review for the clinical significance for all variants in this submission.  
+If your organization has already been approved as an expert panel or practice guideline group (http://www.ncbi.nlm.nih.gov/clinvar/docs/review_guidelines/), please indicate the review status of this submission. Review status of all other submissions will be calculated by ClinVar.  </t>
+  </si>
 </sst>
 </file>
 
@@ -483,7 +792,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -567,6 +876,25 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF0000FF"/>
+      <name val="Geneva"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -635,7 +963,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -725,6 +1053,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -737,7 +1089,7 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -747,10 +1099,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1008,10 +1356,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1122,6 +1466,135 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Accent5 2" xfId="4"/>
@@ -1475,6 +1948,461 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AB11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="1:28">
+      <c r="A2" s="132" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="133"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="136"/>
+      <c r="M2" s="136"/>
+      <c r="N2" s="136"/>
+      <c r="O2" s="136"/>
+      <c r="P2" s="136"/>
+      <c r="Q2" s="136"/>
+      <c r="R2" s="136"/>
+      <c r="S2" s="136"/>
+      <c r="T2" s="136"/>
+      <c r="U2" s="137"/>
+      <c r="V2" s="136"/>
+      <c r="W2" s="135"/>
+      <c r="X2" s="135"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="128"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="6"/>
+    </row>
+    <row r="3" spans="1:28">
+      <c r="A3" s="138" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="139"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="135"/>
+      <c r="H3" s="135"/>
+      <c r="I3" s="135"/>
+      <c r="J3" s="135"/>
+      <c r="K3" s="136"/>
+      <c r="L3" s="136"/>
+      <c r="M3" s="136"/>
+      <c r="N3" s="136"/>
+      <c r="O3" s="136"/>
+      <c r="P3" s="136"/>
+      <c r="Q3" s="136"/>
+      <c r="R3" s="136"/>
+      <c r="S3" s="136"/>
+      <c r="T3" s="136"/>
+      <c r="U3" s="137"/>
+      <c r="V3" s="136"/>
+      <c r="W3" s="135"/>
+      <c r="X3" s="135"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="128"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="6"/>
+    </row>
+    <row r="4" spans="1:28">
+      <c r="A4" s="141" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="142"/>
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="135"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="135"/>
+      <c r="H4" s="135"/>
+      <c r="I4" s="135"/>
+      <c r="J4" s="135"/>
+      <c r="K4" s="136"/>
+      <c r="L4" s="136"/>
+      <c r="M4" s="136"/>
+      <c r="N4" s="136"/>
+      <c r="O4" s="136"/>
+      <c r="P4" s="136"/>
+      <c r="Q4" s="136"/>
+      <c r="R4" s="136"/>
+      <c r="S4" s="136"/>
+      <c r="T4" s="136"/>
+      <c r="U4" s="137"/>
+      <c r="V4" s="136"/>
+      <c r="W4" s="135"/>
+      <c r="X4" s="135"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="128"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="6"/>
+    </row>
+    <row r="5" spans="1:28">
+      <c r="A5" s="143" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="144"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="145"/>
+      <c r="E5" s="146"/>
+      <c r="F5" s="147"/>
+      <c r="G5" s="146"/>
+      <c r="H5" s="146"/>
+      <c r="I5" s="146"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="147"/>
+      <c r="L5" s="147"/>
+      <c r="M5" s="147"/>
+      <c r="N5" s="147"/>
+      <c r="O5" s="147"/>
+      <c r="P5" s="147"/>
+      <c r="Q5" s="147"/>
+      <c r="R5" s="147"/>
+      <c r="S5" s="147"/>
+      <c r="T5" s="147"/>
+      <c r="U5" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="V5" s="148"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="149"/>
+      <c r="AA5" s="17"/>
+      <c r="AB5" s="18"/>
+    </row>
+    <row r="6" spans="1:28" ht="49">
+      <c r="A6" s="150" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="J6" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="K6" s="150" t="s">
+        <v>128</v>
+      </c>
+      <c r="L6" s="150" t="s">
+        <v>129</v>
+      </c>
+      <c r="M6" s="150" t="s">
+        <v>130</v>
+      </c>
+      <c r="N6" s="150" t="s">
+        <v>131</v>
+      </c>
+      <c r="O6" s="150" t="s">
+        <v>132</v>
+      </c>
+      <c r="P6" s="150" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q6" s="150" t="s">
+        <v>134</v>
+      </c>
+      <c r="R6" s="150" t="s">
+        <v>135</v>
+      </c>
+      <c r="S6" s="150" t="s">
+        <v>136</v>
+      </c>
+      <c r="T6" s="150" t="s">
+        <v>137</v>
+      </c>
+      <c r="U6" s="151" t="s">
+        <v>138</v>
+      </c>
+      <c r="V6" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="W6" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="X6" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y6" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z6" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA6" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB6" s="32" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="409">
+      <c r="A7" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="F7" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="G7" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="H7" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="I7" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="K7" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="L7" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="M7" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="N7" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="O7" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="P7" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q7" s="37" t="s">
+        <v>161</v>
+      </c>
+      <c r="R7" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="S7" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="T7" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="U7" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="V7" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="W7" s="42" t="s">
+        <v>193</v>
+      </c>
+      <c r="X7" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y7" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z7" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="AA7" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="AB7" s="38" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="16" thickBot="1">
+      <c r="A8" s="152" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" s="153"/>
+      <c r="C8" s="154"/>
+      <c r="D8" s="154"/>
+      <c r="E8" s="154"/>
+      <c r="F8" s="155"/>
+      <c r="G8" s="154"/>
+      <c r="H8" s="154"/>
+      <c r="I8" s="154"/>
+      <c r="J8" s="154"/>
+      <c r="K8" s="155"/>
+      <c r="L8" s="155"/>
+      <c r="M8" s="155"/>
+      <c r="N8" s="155"/>
+      <c r="O8" s="155"/>
+      <c r="P8" s="155"/>
+      <c r="Q8" s="155"/>
+      <c r="R8" s="155"/>
+      <c r="S8" s="155"/>
+      <c r="T8" s="155"/>
+      <c r="U8" s="156"/>
+      <c r="V8" s="155"/>
+      <c r="W8" s="154"/>
+      <c r="X8" s="154"/>
+      <c r="Y8" s="154"/>
+      <c r="Z8" s="157"/>
+      <c r="AA8" s="154"/>
+      <c r="AB8" s="158"/>
+    </row>
+    <row r="9" spans="1:28" ht="50" thickTop="1">
+      <c r="A9" s="159" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" s="160" t="s">
+        <v>172</v>
+      </c>
+      <c r="C9" s="160" t="s">
+        <v>173</v>
+      </c>
+      <c r="D9" s="160" t="s">
+        <v>174</v>
+      </c>
+      <c r="E9" s="160" t="s">
+        <v>175</v>
+      </c>
+      <c r="F9" s="159" t="s">
+        <v>176</v>
+      </c>
+      <c r="G9" s="86" t="s">
+        <v>177</v>
+      </c>
+      <c r="H9" s="86" t="s">
+        <v>178</v>
+      </c>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86" t="s">
+        <v>179</v>
+      </c>
+      <c r="K9" s="161">
+        <v>500000</v>
+      </c>
+      <c r="L9" s="161"/>
+      <c r="M9" s="161"/>
+      <c r="N9" s="161" t="s">
+        <v>180</v>
+      </c>
+      <c r="O9" s="161" t="s">
+        <v>181</v>
+      </c>
+      <c r="P9" s="161" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q9" s="161" t="s">
+        <v>183</v>
+      </c>
+      <c r="R9" s="161" t="s">
+        <v>184</v>
+      </c>
+      <c r="S9" s="162" t="s">
+        <v>185</v>
+      </c>
+      <c r="T9" s="162"/>
+      <c r="U9" s="163"/>
+      <c r="V9" s="162"/>
+      <c r="W9" s="86"/>
+      <c r="X9" s="86" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y9" s="86"/>
+      <c r="Z9" s="164"/>
+      <c r="AA9" s="86"/>
+      <c r="AB9" s="87" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="26" thickBot="1">
+      <c r="A10" s="165" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" s="166" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" s="167"/>
+      <c r="D10" s="167"/>
+      <c r="E10" s="167"/>
+      <c r="F10" s="168"/>
+      <c r="G10" s="167"/>
+      <c r="H10" s="167"/>
+      <c r="I10" s="167"/>
+      <c r="J10" s="167"/>
+      <c r="K10" s="168"/>
+      <c r="L10" s="168"/>
+      <c r="M10" s="168"/>
+      <c r="N10" s="168"/>
+      <c r="O10" s="168"/>
+      <c r="P10" s="168"/>
+      <c r="Q10" s="168"/>
+      <c r="R10" s="168"/>
+      <c r="S10" s="168"/>
+      <c r="T10" s="168"/>
+      <c r="U10" s="169"/>
+      <c r="V10" s="168"/>
+      <c r="W10" s="167"/>
+      <c r="X10" s="167"/>
+      <c r="Y10" s="170"/>
+      <c r="Z10" s="171"/>
+      <c r="AA10" s="170"/>
+      <c r="AB10" s="167"/>
+    </row>
+    <row r="11" spans="1:28" ht="16" thickTop="1"/>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1487,427 +2415,427 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="2" t="s">
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
     </row>
     <row r="2" spans="1:26" ht="49">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="20" t="s">
+      <c r="F2" s="14"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="23" t="s">
+      <c r="P2" s="20"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="24"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
     </row>
     <row r="3" spans="1:26" ht="73">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="I3" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="31" t="s">
+      <c r="J3" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="L3" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="27" t="s">
+      <c r="M3" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="27" t="s">
+      <c r="N3" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="32" t="s">
+      <c r="O3" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="P3" s="33" t="s">
+      <c r="P3" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="34" t="s">
+      <c r="Q3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="33" t="s">
+      <c r="R3" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="S3" s="33" t="s">
+      <c r="S3" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="T3" s="33" t="s">
+      <c r="T3" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="U3" s="33" t="s">
+      <c r="U3" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="33" t="s">
+      <c r="V3" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="W3" s="35" t="s">
+      <c r="W3" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="X3" s="33" t="s">
+      <c r="X3" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="Y3" s="33" t="s">
+      <c r="Y3" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="Z3" s="33" t="s">
+      <c r="Z3" s="32" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="409">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="H4" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="42" t="s">
+      <c r="I4" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="43" t="s">
+      <c r="J4" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="43" t="s">
+      <c r="K4" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="L4" s="43" t="s">
+      <c r="L4" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="M4" s="44" t="s">
+      <c r="M4" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="N4" s="43" t="s">
+      <c r="N4" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="O4" s="45" t="s">
+      <c r="O4" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="P4" s="43" t="s">
+      <c r="P4" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" s="41" t="s">
+      <c r="Q4" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="R4" s="43" t="s">
+      <c r="R4" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="S4" s="43" t="s">
+      <c r="S4" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="43" t="s">
+      <c r="T4" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="U4" s="43" t="s">
+      <c r="U4" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="V4" s="46" t="s">
+      <c r="V4" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="W4" s="43" t="s">
+      <c r="W4" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="X4" s="43" t="s">
+      <c r="X4" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="Y4" s="43" t="s">
+      <c r="Y4" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="Z4" s="43" t="s">
+      <c r="Z4" s="42" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="16" thickBot="1">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="55"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="52"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="50"/>
-      <c r="T5" s="50"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="56"/>
-      <c r="W5" s="56"/>
-      <c r="X5" s="57"/>
-      <c r="Y5" s="56"/>
-      <c r="Z5" s="56"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="49"/>
+      <c r="U5" s="49"/>
+      <c r="V5" s="55"/>
+      <c r="W5" s="55"/>
+      <c r="X5" s="56"/>
+      <c r="Y5" s="55"/>
+      <c r="Z5" s="55"/>
     </row>
     <row r="6" spans="1:26" ht="16" thickTop="1">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="60" t="s">
+      <c r="B6" s="58"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="60" t="s">
+      <c r="E6" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="61">
+      <c r="F6" s="60">
         <v>41306</v>
       </c>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="63" t="s">
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="64"/>
-      <c r="N6" s="64"/>
-      <c r="O6" s="64"/>
-      <c r="P6" s="64"/>
-      <c r="Q6" s="64"/>
-      <c r="R6" s="65" t="s">
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="63"/>
+      <c r="R6" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="S6" s="66"/>
-      <c r="T6" s="67"/>
-      <c r="U6" s="67"/>
-      <c r="V6" s="67"/>
-      <c r="W6" s="67"/>
-      <c r="X6" s="67"/>
-      <c r="Y6" s="67"/>
-      <c r="Z6" s="67"/>
+      <c r="S6" s="65"/>
+      <c r="T6" s="66"/>
+      <c r="U6" s="66"/>
+      <c r="V6" s="66"/>
+      <c r="W6" s="66"/>
+      <c r="X6" s="66"/>
+      <c r="Y6" s="66"/>
+      <c r="Z6" s="66"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="69" t="s">
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="68" t="s">
+      <c r="E7" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="70">
+      <c r="F7" s="69">
         <v>41306</v>
       </c>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="68" t="s">
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="72"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="73"/>
-      <c r="N7" s="73"/>
-      <c r="O7" s="73"/>
-      <c r="P7" s="73"/>
-      <c r="Q7" s="73"/>
-      <c r="R7" s="72" t="s">
+      <c r="J7" s="71"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="72"/>
+      <c r="M7" s="72"/>
+      <c r="N7" s="72"/>
+      <c r="O7" s="72"/>
+      <c r="P7" s="72"/>
+      <c r="Q7" s="72"/>
+      <c r="R7" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="S7" s="74"/>
-      <c r="T7" s="74"/>
-      <c r="U7" s="74"/>
-      <c r="V7" s="75"/>
-      <c r="W7" s="75"/>
-      <c r="X7" s="74"/>
-      <c r="Y7" s="74"/>
-      <c r="Z7" s="74"/>
+      <c r="S7" s="73"/>
+      <c r="T7" s="73"/>
+      <c r="U7" s="73"/>
+      <c r="V7" s="74"/>
+      <c r="W7" s="74"/>
+      <c r="X7" s="73"/>
+      <c r="Y7" s="73"/>
+      <c r="Z7" s="73"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="76"/>
-      <c r="E8" s="69" t="s">
+      <c r="D8" s="75"/>
+      <c r="E8" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="70">
+      <c r="F8" s="69">
         <v>41306</v>
       </c>
-      <c r="G8" s="71"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="76" t="s">
+      <c r="G8" s="70"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="J8" s="76"/>
-      <c r="K8" s="74"/>
-      <c r="L8" s="74"/>
-      <c r="M8" s="74"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="78"/>
-      <c r="P8" s="74"/>
-      <c r="Q8" s="78"/>
-      <c r="R8" s="76" t="s">
+      <c r="J8" s="75"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="77"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="77"/>
+      <c r="R8" s="75" t="s">
         <v>75</v>
       </c>
-      <c r="S8" s="74"/>
-      <c r="T8" s="74"/>
-      <c r="U8" s="74"/>
-      <c r="V8" s="74"/>
-      <c r="W8" s="74"/>
-      <c r="X8" s="74"/>
-      <c r="Y8" s="74"/>
-      <c r="Z8" s="74"/>
+      <c r="S8" s="73"/>
+      <c r="T8" s="73"/>
+      <c r="U8" s="73"/>
+      <c r="V8" s="73"/>
+      <c r="W8" s="73"/>
+      <c r="X8" s="73"/>
+      <c r="Y8" s="73"/>
+      <c r="Z8" s="73"/>
     </row>
     <row r="9" spans="1:26">
-      <c r="A9" s="79" t="s">
+      <c r="A9" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="79" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="80" t="s">
+      <c r="C9" s="79" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="81"/>
-      <c r="E9" s="79" t="s">
+      <c r="D9" s="80"/>
+      <c r="E9" s="78" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="82">
+      <c r="F9" s="81">
         <v>41306</v>
       </c>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="79" t="s">
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="J9" s="84"/>
-      <c r="K9" s="85"/>
-      <c r="L9" s="85"/>
-      <c r="M9" s="85"/>
-      <c r="N9" s="85"/>
-      <c r="O9" s="85"/>
-      <c r="P9" s="85"/>
-      <c r="Q9" s="85"/>
-      <c r="R9" s="86" t="s">
+      <c r="J9" s="83"/>
+      <c r="K9" s="84"/>
+      <c r="L9" s="84"/>
+      <c r="M9" s="84"/>
+      <c r="N9" s="84"/>
+      <c r="O9" s="84"/>
+      <c r="P9" s="84"/>
+      <c r="Q9" s="84"/>
+      <c r="R9" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="S9" s="87"/>
-      <c r="T9" s="87"/>
-      <c r="U9" s="88"/>
-      <c r="V9" s="88"/>
-      <c r="W9" s="88"/>
-      <c r="X9" s="88"/>
-      <c r="Y9" s="88"/>
-      <c r="Z9" s="88"/>
+      <c r="S9" s="86"/>
+      <c r="T9" s="86"/>
+      <c r="U9" s="87"/>
+      <c r="V9" s="87"/>
+      <c r="W9" s="87"/>
+      <c r="X9" s="87"/>
+      <c r="Y9" s="87"/>
+      <c r="Z9" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1926,7 +2854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
@@ -1936,301 +2864,301 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="7" width="29" style="6" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="37.1640625" style="130" customWidth="1"/>
-    <col min="10" max="10" width="30.5" style="6" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" style="6" customWidth="1"/>
-    <col min="13" max="14" width="21.1640625" style="6" customWidth="1"/>
-    <col min="15" max="15" width="21.5" style="6" customWidth="1"/>
-    <col min="16" max="16" width="20.1640625" style="6" customWidth="1"/>
-    <col min="17" max="16384" width="8.83203125" style="6"/>
+    <col min="1" max="7" width="29" style="5" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="37.1640625" style="128" customWidth="1"/>
+    <col min="10" max="10" width="30.5" style="5" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" style="5" customWidth="1"/>
+    <col min="13" max="14" width="21.1640625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="21.5" style="5" customWidth="1"/>
+    <col min="16" max="16" width="20.1640625" style="5" customWidth="1"/>
+    <col min="17" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="91" customFormat="1">
-      <c r="A1" s="89" t="s">
+    <row r="1" spans="1:16" s="89" customFormat="1">
+      <c r="A1" s="131" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="I1" s="92"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="I1" s="90"/>
     </row>
-    <row r="2" spans="1:16" s="101" customFormat="1">
-      <c r="A2" s="93" t="s">
+    <row r="2" spans="1:16" s="99" customFormat="1">
+      <c r="A2" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="96" t="s">
+      <c r="C2" s="93"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="94" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="97"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="100"/>
-      <c r="O2" s="100"/>
-      <c r="P2" s="100"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
     </row>
     <row r="3" spans="1:16" ht="37">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="102" t="s">
+      <c r="F3" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="103" t="s">
+      <c r="H3" s="101" t="s">
         <v>85</v>
       </c>
-      <c r="I3" s="34" t="s">
+      <c r="I3" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="L3" s="104" t="s">
+      <c r="L3" s="102" t="s">
         <v>89</v>
       </c>
-      <c r="M3" s="104" t="s">
+      <c r="M3" s="102" t="s">
         <v>90</v>
       </c>
-      <c r="N3" s="35" t="s">
+      <c r="N3" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="33" t="s">
+      <c r="O3" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="P3" s="34" t="s">
+      <c r="P3" s="33" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="204">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="I4" s="41" t="s">
+      <c r="I4" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="J4" s="43" t="s">
+      <c r="J4" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="K4" s="105" t="s">
+      <c r="K4" s="103" t="s">
         <v>102</v>
       </c>
-      <c r="L4" s="106" t="s">
+      <c r="L4" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="M4" s="106" t="s">
+      <c r="M4" s="104" t="s">
         <v>104</v>
       </c>
-      <c r="N4" s="43" t="s">
+      <c r="N4" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="O4" s="43" t="s">
+      <c r="O4" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="P4" s="41" t="s">
+      <c r="P4" s="40" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="110" customFormat="1" ht="16" thickBot="1">
-      <c r="A5" s="107" t="s">
+    <row r="5" spans="1:16" s="108" customFormat="1" ht="16" thickBot="1">
+      <c r="A5" s="105" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="109"/>
-      <c r="J5" s="108"/>
-      <c r="K5" s="108"/>
-      <c r="L5" s="108"/>
-      <c r="M5" s="108"/>
-      <c r="N5" s="108"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="106"/>
+      <c r="K5" s="106"/>
+      <c r="L5" s="106"/>
+      <c r="M5" s="106"/>
+      <c r="N5" s="106"/>
     </row>
-    <row r="6" spans="1:16" s="116" customFormat="1" ht="16" thickTop="1">
-      <c r="A6" s="111"/>
-      <c r="B6" s="112"/>
-      <c r="C6" s="113"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="111"/>
-      <c r="G6" s="114"/>
-      <c r="H6" s="111"/>
-      <c r="I6" s="115"/>
-      <c r="J6" s="111"/>
-      <c r="K6" s="111"/>
-      <c r="L6" s="114"/>
-      <c r="M6" s="114"/>
-      <c r="N6" s="111"/>
+    <row r="6" spans="1:16" s="114" customFormat="1" ht="16" thickTop="1">
+      <c r="A6" s="109"/>
+      <c r="B6" s="110"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="112"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="113"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="112"/>
+      <c r="M6" s="112"/>
+      <c r="N6" s="109"/>
     </row>
-    <row r="7" spans="1:16" s="116" customFormat="1">
-      <c r="A7" s="111"/>
-      <c r="B7" s="117"/>
-      <c r="C7" s="118"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="114"/>
-      <c r="G7" s="114"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="115"/>
-      <c r="J7" s="111"/>
-      <c r="K7" s="111"/>
-      <c r="L7" s="114"/>
-      <c r="M7" s="114"/>
-      <c r="N7" s="111"/>
+    <row r="7" spans="1:16" s="114" customFormat="1">
+      <c r="A7" s="109"/>
+      <c r="B7" s="115"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="112"/>
+      <c r="G7" s="112"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="113"/>
+      <c r="J7" s="109"/>
+      <c r="K7" s="109"/>
+      <c r="L7" s="112"/>
+      <c r="M7" s="112"/>
+      <c r="N7" s="109"/>
     </row>
-    <row r="8" spans="1:16" s="116" customFormat="1">
-      <c r="A8" s="119" t="s">
+    <row r="8" spans="1:16" s="114" customFormat="1">
+      <c r="A8" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="77"/>
-      <c r="C8" s="119"/>
-      <c r="D8" s="120" t="s">
+      <c r="B8" s="76"/>
+      <c r="C8" s="117"/>
+      <c r="D8" s="118" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="120"/>
-      <c r="F8" s="121" t="s">
+      <c r="E8" s="118"/>
+      <c r="F8" s="119" t="s">
         <v>109</v>
       </c>
-      <c r="G8" s="121" t="s">
+      <c r="G8" s="119" t="s">
         <v>110</v>
       </c>
-      <c r="H8" s="122"/>
-      <c r="I8" s="122"/>
-      <c r="J8" s="122"/>
-      <c r="K8" s="122"/>
-      <c r="L8" s="121"/>
-      <c r="M8" s="121"/>
-      <c r="N8" s="122"/>
+      <c r="H8" s="120"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="120"/>
+      <c r="K8" s="120"/>
+      <c r="L8" s="119"/>
+      <c r="M8" s="119"/>
+      <c r="N8" s="120"/>
     </row>
-    <row r="9" spans="1:16" s="116" customFormat="1">
-      <c r="A9" s="123" t="s">
+    <row r="9" spans="1:16" s="114" customFormat="1">
+      <c r="A9" s="121" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="123"/>
-      <c r="C9" s="123"/>
-      <c r="D9" s="119" t="s">
+      <c r="B9" s="121"/>
+      <c r="C9" s="121"/>
+      <c r="D9" s="117" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="119"/>
-      <c r="F9" s="121" t="s">
+      <c r="E9" s="117"/>
+      <c r="F9" s="119" t="s">
         <v>109</v>
       </c>
-      <c r="G9" s="121" t="s">
+      <c r="G9" s="119" t="s">
         <v>110</v>
       </c>
-      <c r="H9" s="122"/>
-      <c r="I9" s="122"/>
-      <c r="J9" s="122"/>
-      <c r="K9" s="122"/>
-      <c r="L9" s="121"/>
-      <c r="M9" s="121"/>
-      <c r="N9" s="122"/>
+      <c r="H9" s="120"/>
+      <c r="I9" s="120"/>
+      <c r="J9" s="120"/>
+      <c r="K9" s="120"/>
+      <c r="L9" s="119"/>
+      <c r="M9" s="119"/>
+      <c r="N9" s="120"/>
     </row>
-    <row r="10" spans="1:16" s="126" customFormat="1">
-      <c r="A10" s="124" t="s">
+    <row r="10" spans="1:16" s="124" customFormat="1">
+      <c r="A10" s="122" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="125"/>
-      <c r="E10" s="125"/>
-      <c r="F10" s="121" t="s">
+      <c r="D10" s="123"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="119" t="s">
         <v>109</v>
       </c>
-      <c r="G10" s="121" t="s">
+      <c r="G10" s="119" t="s">
         <v>110</v>
       </c>
-      <c r="H10" s="122"/>
-      <c r="I10" s="122"/>
-      <c r="J10" s="122"/>
-      <c r="K10" s="122"/>
-      <c r="L10" s="121"/>
-      <c r="M10" s="121"/>
-      <c r="N10" s="122"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="120"/>
+      <c r="K10" s="120"/>
+      <c r="L10" s="119"/>
+      <c r="M10" s="119"/>
+      <c r="N10" s="120"/>
     </row>
-    <row r="11" spans="1:16" s="129" customFormat="1">
-      <c r="A11" s="127" t="s">
+    <row r="11" spans="1:16" s="127" customFormat="1">
+      <c r="A11" s="125" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="79" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="80" t="s">
+      <c r="C11" s="79" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="128"/>
-      <c r="E11" s="128"/>
-      <c r="F11" s="128" t="s">
+      <c r="D11" s="126"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126" t="s">
         <v>109</v>
       </c>
-      <c r="G11" s="128" t="s">
+      <c r="G11" s="126" t="s">
         <v>110</v>
       </c>
-      <c r="H11" s="128"/>
-      <c r="I11" s="128"/>
-      <c r="J11" s="128"/>
-      <c r="K11" s="128"/>
-      <c r="L11" s="128"/>
-      <c r="M11" s="128"/>
-      <c r="N11" s="128"/>
+      <c r="H11" s="126"/>
+      <c r="I11" s="126"/>
+      <c r="J11" s="126"/>
+      <c r="K11" s="126"/>
+      <c r="L11" s="126"/>
+      <c r="M11" s="126"/>
+      <c r="N11" s="126"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2262,11 +3190,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2277,23 +3205,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="129" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="60">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="45" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>